<commit_message>
Comparing with experimental results
</commit_message>
<xml_diff>
--- a/Weibull_constants_diagonals_vary_Height1.xlsx
+++ b/Weibull_constants_diagonals_vary_Height1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtan15\Documents\GitHub\Monte-Carlos-MgO-TDDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE066DE-BB36-4FD3-8F57-82DC58ED8E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CA6BEB-1273-4AD2-AF9B-296D1AF295B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -732,7 +732,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection sqref="A1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -781,44 +781,44 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
-        <f>1/(50*0.0002*A2^-27.15)</f>
-        <v>18.638940640328606</v>
+        <f>1/(235*0.0002*A2^-27.15)</f>
+        <v>3.965732051133747</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:J4" si="0">1/(50*0.0002*B2^-27.15)</f>
-        <v>10.395359485927873</v>
+        <f t="shared" ref="B4:J4" si="0">1/(235*0.0002*B2^-27.15)</f>
+        <v>2.2117786140272071</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>5.7237957952712692</v>
+        <v>1.2178288926109084</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>3.1096001521802221</v>
+        <v>0.66161705365536638</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>1.6658387155992811</v>
+        <v>0.35443376927644282</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0.87939221491977926</v>
+        <v>0.18710472657867644</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>0.45713670353195318</v>
+        <v>9.7263128411053876E-2</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>0.23382618654069035</v>
+        <v>4.9750252455466028E-2</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>0.11758947815797942</v>
+        <v>2.5019037905953067E-2</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>5.8088348650420674E-2</v>
+        <v>1.2359223117110784E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>